<commit_message>
- Fixed generating Today date fields. - Fixed audit code: Added RECORDNUMBER field. - Added emptying hidden fields for hide code. - Fixed some minor display issues.
</commit_message>
<xml_diff>
--- a/EpiData/datadict.xlsx
+++ b/EpiData/datadict.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -879,11 +879,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC864245-278E-43A2-9E7C-BDBB7FF6F5C6}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1523,7 +1523,7 @@
   <conditionalFormatting sqref="B15:B17">
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C17" xr:uid="{70305254-47A4-4525-857A-4B24F3AD8FAB}">
       <formula1>"bin,date,id,nom,quan,text"</formula1>
     </dataValidation>
@@ -1540,7 +1540,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0D88DE45-6C8C-4873-B89A-79FB806AC9BA}">
           <x14:formula1>
             <xm:f>_xlfn.ANCHORARRAY(settings!$A$2)</xm:f>
@@ -1557,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2333AF4C-E470-4402-8B0D-BCB0B14E4108}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>